<commit_message>
Cleaned up text and spell checked
</commit_message>
<xml_diff>
--- a/LDRD_RomanPots-Budget.xlsx
+++ b/LDRD_RomanPots-Budget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2030" yWindow="60" windowWidth="11360" windowHeight="10850"/>
+    <workbookView xWindow="2030" yWindow="60" windowWidth="11360" windowHeight="10850" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -239,9 +239,6 @@
     <t>indirect rates columns.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Postdoc Kansas</t>
-  </si>
-  <si>
     <t>Travel</t>
   </si>
   <si>
@@ -254,14 +251,20 @@
     <t>Alexandre Camsonne</t>
   </si>
   <si>
-    <t>Roman pot R&amp;D</t>
+    <t>Student Kansas</t>
+  </si>
+  <si>
+    <t>Study of feasibility and preliminary design of roman pots for the JLAB EIC</t>
+  </si>
+  <si>
+    <t>STUDY OF FEASIBILITY AND PRELIMINARY DESIGN OF ROMAN POTS FOR THE JLAB EIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +407,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -902,9 +911,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1066,6 +1072,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1370,72 +1377,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.54296875" style="3" customWidth="1"/>
-    <col min="2" max="4" width="7.54296875" style="44" customWidth="1"/>
+    <col min="2" max="4" width="7.54296875" style="43" customWidth="1"/>
     <col min="5" max="6" width="15.54296875" customWidth="1"/>
     <col min="7" max="7" width="14.453125" customWidth="1"/>
     <col min="8" max="8" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="74"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="29"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="42" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76"/>
+      <c r="F2" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="75"/>
     </row>
     <row r="3" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="70" t="s">
+      <c r="C3" s="82"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
+      <c r="F3" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="76"/>
+      <c r="H3" s="77"/>
     </row>
     <row r="4" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="44" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1447,7 +1454,7 @@
       <c r="G4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="31" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="3"/>
@@ -1460,9 +1467,9 @@
       <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1473,110 +1480,111 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="6">
-        <v>4</v>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6">
+        <f>90782*0.05</f>
+        <v>4539.1000000000004</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="21">
         <f>SUM(E6:G6)</f>
-        <v>4</v>
+        <v>4539.1000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="6">
-        <v>20</v>
+        <v>15000</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="21">
         <f t="shared" ref="H7:H9" si="0">SUM(E7:G7)</f>
-        <v>20</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="67">
         <v>0.51300000000000001</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="67">
         <v>0.51300000000000001</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="67">
         <v>0.51300000000000001</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="50">
         <f>ROUND(E6*B8,0)</f>
-        <v>2</v>
-      </c>
-      <c r="F8" s="51">
+        <v>2329</v>
+      </c>
+      <c r="F8" s="50">
         <f>ROUND(F6*C8,0)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="50">
         <f>ROUND(G6*D8,0)</f>
         <v>0</v>
       </c>
       <c r="H8" s="21">
         <f>SUM((E8:G8))</f>
-        <v>2</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="68">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="C9" s="69">
+      <c r="C9" s="68">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="68">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="50">
         <f>ROUND((E6+E7)*B9,0)</f>
-        <v>2</v>
-      </c>
-      <c r="F9" s="51">
+        <v>1739</v>
+      </c>
+      <c r="F9" s="50">
         <f t="shared" ref="F9:G9" si="1">ROUND((F6+F7)*C9,0)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9" s="21">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="39" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="38" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="9">
         <f>SUM(E6:E9)</f>
-        <v>28</v>
+        <v>23607.1</v>
       </c>
       <c r="F10" s="9">
         <f>SUM(F6:F9)</f>
@@ -1586,35 +1594,35 @@
         <f>SUM(G6:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="37">
         <f>SUM(E10:G10)</f>
-        <v>28</v>
+        <v>23607.1</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="6">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="21">
         <f>SUM(E11:G11)</f>
-        <v>10</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1627,9 +1635,9 @@
       <c r="A13" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1642,9 +1650,9 @@
       <c r="A14" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1657,9 +1665,9 @@
       <c r="A15" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1672,9 +1680,9 @@
       <c r="A16" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -1687,12 +1695,12 @@
       <c r="A17" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
       <c r="E17" s="9">
         <f>SUM(E10:E16)</f>
-        <v>38</v>
+        <v>33607.1</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" ref="F17:G17" si="3">SUM(F10:F16)</f>
@@ -1704,16 +1712,16 @@
       </c>
       <c r="H17" s="24">
         <f>SUM(E17:G17)</f>
-        <v>38</v>
+        <v>33607.1</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="7" t="s">
         <v>9</v>
       </c>
@@ -1725,66 +1733,66 @@
       <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="69">
+      <c r="B19" s="68">
         <v>0.49199999999999999</v>
       </c>
-      <c r="C19" s="69">
+      <c r="C19" s="68">
         <v>0.49199999999999999</v>
       </c>
-      <c r="D19" s="69">
+      <c r="D19" s="68">
         <v>0.54</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="50">
         <f>ROUND(((E10+E11+E12+E13+E14+E15)*B19),0)</f>
-        <v>19</v>
-      </c>
-      <c r="F19" s="51">
+        <v>16535</v>
+      </c>
+      <c r="F19" s="50">
         <f t="shared" ref="F19:G19" si="4">ROUND(((F10+F11+F12+F13+F14+F15)*C19),0)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" ref="H19:H20" si="5">SUM(E19:G19)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16535</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="40" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="40">
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="39">
         <f>SUM(E19:E19)</f>
-        <v>19</v>
-      </c>
-      <c r="F20" s="40">
+        <v>16535</v>
+      </c>
+      <c r="F20" s="39">
         <f t="shared" ref="F20:G20" si="6">SUM(F19:F19)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="39">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="37">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>16535</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
       <c r="E21" s="9">
         <f>SUM(E17+E20)</f>
-        <v>57</v>
+        <v>50142.1</v>
       </c>
       <c r="F21" s="9">
         <f>SUM(F17+F20)</f>
@@ -1796,68 +1804,68 @@
       </c>
       <c r="H21" s="28">
         <f>SUM(E21:G21)</f>
-        <v>57</v>
+        <v>50142.1</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="28">
         <f>SUM(H21+H22)</f>
-        <v>57</v>
+        <v>50142.1</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1878,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1889,18 +1897,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="74"/>
+      <c r="B1" s="73"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="91"/>
+      <c r="B2" s="90"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="3"/>
@@ -1908,163 +1916,167 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="89"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30"/>
+      <c r="B5" s="91" t="s">
+        <v>61</v>
+      </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="86" t="s">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="87"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="19"/>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="33">
-        <v>20</v>
+      <c r="B9">
+        <f>90782*0.05</f>
+        <v>4539.1000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="33">
-        <v>4.45</v>
+      <c r="B10" s="32">
+        <v>15000</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="62"/>
+      <c r="B11" s="61"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="61"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="33">
-        <v>5</v>
+      <c r="B13" s="32">
+        <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="32"/>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="32"/>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="32"/>
     </row>
     <row r="17" spans="1:2" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="32"/>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="32"/>
+    </row>
+    <row r="19" spans="1:2" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="33">
+        <f>SUM(B9:B18)</f>
+        <v>29539.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="19"/>
+    </row>
+    <row r="21" spans="1:2" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="61" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="63" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="33"/>
-    </row>
-    <row r="19" spans="1:2" s="1" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="34"/>
-    </row>
-    <row r="20" spans="1:2" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="19"/>
-    </row>
-    <row r="21" spans="1:2" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="62" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
     </row>
     <row r="23" spans="1:2" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="36"/>
     </row>
     <row r="24" spans="1:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
     </row>
     <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="85" t="s">
+      <c r="A25" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="85"/>
+      <c r="B25" s="84"/>
     </row>
     <row r="26" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="71"/>
+      <c r="B26" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2095,28 +2107,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
+      <c r="A2" s="52"/>
     </row>
     <row r="3" spans="1:1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="54"/>
     </row>
     <row r="5" spans="1:1" ht="174" x14ac:dyDescent="0.35">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="54" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="56"/>
+      <c r="A6" s="55"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2130,42 +2142,43 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C1">
-        <v>20</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2">
-        <v>4.45</v>
+        <f>90782*0.05</f>
+        <v>4539.1000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <f>SUM(C1:C3)</f>
-        <v>29.45</v>
+        <v>29539.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>